<commit_message>
Add upcountry invoice id into booking details
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anujaggarwal/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anujaggarwal/Downloads/templates/anuj/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>TIN: 07627112651</t>
   </si>
@@ -74,12 +74,6 @@
     <t>BILL TO:</t>
   </si>
   <si>
-    <t>Vendor Number: 252752</t>
-  </si>
-  <si>
-    <t>Seller Code: S9f330</t>
-  </si>
-  <si>
     <t>ANNEXURE</t>
   </si>
   <si>
@@ -114,6 +108,9 @@
   </si>
   <si>
     <t>{booking:remarks}</t>
+  </si>
+  <si>
+    <t>{meta:seller_code}</t>
   </si>
 </sst>
 </file>
@@ -182,15 +179,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -244,28 +232,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="medium">
         <color auto="1"/>
@@ -288,6 +254,43 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -307,83 +310,83 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,7 +695,7 @@
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -710,190 +713,188 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24"/>
+    </row>
+    <row r="7" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="13"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="9"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="24"/>
+    </row>
+    <row r="12" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="26"/>
-    </row>
-    <row r="8" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="14"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="26"/>
-    </row>
-    <row r="9" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="10"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="26"/>
-    </row>
-    <row r="10" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="18" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="26"/>
-    </row>
-    <row r="11" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="15" t="s">
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="18"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="24"/>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="18"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="24"/>
+    </row>
+    <row r="15" spans="2:7" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18" t="s">
+      <c r="C16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="26"/>
-    </row>
-    <row r="13" spans="2:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="19"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="26"/>
-    </row>
-    <row r="14" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="19"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="26"/>
-    </row>
-    <row r="15" spans="2:7" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="E16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="F16" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="G16" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="17" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="29"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="26"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
Added rating in partner annexure
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>TIN: 07627112651</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>{booking:name}</t>
+  </si>
+  <si>
+    <t>{booking:rating_stars}</t>
+  </si>
+  <si>
+    <t>Rating</t>
   </si>
 </sst>
 </file>
@@ -146,35 +152,41 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -399,9 +411,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -414,6 +423,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,17 +444,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -741,10 +753,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J17"/>
+  <dimension ref="B1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -753,32 +765,34 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="7" width="14.5" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="30.5" style="3" customWidth="1"/>
-    <col min="11" max="11" width="4.1640625" customWidth="1"/>
+    <col min="9" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="24" t="s">
+      <c r="J1" s="1"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="26"/>
-    </row>
-    <row r="3" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
+    </row>
+    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -787,9 +801,10 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
@@ -800,10 +815,11 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="29" t="s">
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="5"/>
@@ -812,13 +828,14 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="30" t="s">
+      <c r="I5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="29" t="s">
+      <c r="J5" s="24"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5"/>
@@ -827,13 +844,14 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="18"/>
-    </row>
-    <row r="7" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="29" t="s">
+      <c r="J6" s="24"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5"/>
@@ -842,12 +860,13 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="18"/>
-    </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J7" s="24"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="8"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -855,12 +874,13 @@
       <c r="F8" s="10"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="18"/>
-    </row>
-    <row r="9" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J8" s="24"/>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -869,9 +889,10 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="18"/>
-    </row>
-    <row r="10" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J9" s="5"/>
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="11" t="s">
         <v>14</v>
       </c>
@@ -884,9 +905,10 @@
       <c r="I10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J10" s="12"/>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
@@ -899,37 +921,40 @@
       <c r="I11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="27" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="18"/>
+    </row>
+    <row r="13" spans="2:11" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J13" s="12"/>
+      <c r="K13" s="18"/>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="13"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -938,38 +963,42 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="2:10" ht="26" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="21" t="s">
+      <c r="J14" s="12"/>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="2:11" ht="26" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="K15" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="14" t="s">
         <v>20</v>
       </c>
@@ -994,11 +1023,14 @@
       <c r="I16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B17" s="16"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -1007,13 +1039,14 @@
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="20"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="19"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="2">
     <mergeCell ref="B12:G13"/>
-    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="42" orientation="portrait"/>

</xml_diff>